<commit_message>
(hel-839) mise en page du texte dans template
</commit_message>
<xml_diff>
--- a/public/templates/template_comparaison_EJ.xlsx
+++ b/public/templates/template_comparaison_EJ.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Debian\home\webadm\projets\helios\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC94AE7D-236C-4E96-AB87-A57CEC936097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F70098A-629F-4F51-9E2F-6AB3DD524889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparaison" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>Indicateurs</t>
   </si>
@@ -32,12 +32,6 @@
     <t>Mise à jour</t>
   </si>
   <si>
-    <t>Statut juridique</t>
-  </si>
-  <si>
-    <t>Rattachements</t>
-  </si>
-  <si>
     <t>Nb de séjours HAD</t>
   </si>
   <si>
@@ -65,69 +59,522 @@
     <t>Allocation de ressources</t>
   </si>
   <si>
-    <t>Source : PMSI
+    <t>date_mis_a_jour_pmsi</t>
+  </si>
+  <si>
+    <t>date_mis_a_jour_ancre</t>
+  </si>
+  <si>
+    <t>date_mis_a_jour_hapi</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Source : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">PMSI
 Permet d’observer l’évolution de l’activité de l’établissement et le développement des prises en charge sur leur lieu de vie de malades atteints de pathologies graves, aiguës ou chroniques.
-Fréquence : Annuelle
-Mode de Calcul : Nombre de séjours commencés lors de la période étudiée (mais pas nécessairement terminés).
-Source(s) :
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Fréquence :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Annuelle
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Mode de Calcul :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Nombre de séjours commencés lors de la période étudiée (mais pas nécessairement terminés).
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Source(s) :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
 Programme de médicalisation des systèmes d’information (PMSI) - Agence technique de l’information sur l’hospitalisation (ATIH)
 Hospitalisation A Domicile (HAD) - fichiers RAPSS (Résumés Anonyme Par Sous-Séquence)
 Hélios collecte ces données depuis le SI mutualisé des ARS DIAMANT « Décisionnel Inter-ARS pour la Maîtrise et l’Anticipation. », outil décisionnel de pilotage centré sur la régulation de l’offre de soins, abordée sous les aspects des moyens humains, financiers, et productivité.
 Dans le cadre du PMSI, tout séjour dans un établissement de santé, public ou privé, fait l’objet d’un recueil systématique et minimal d’informations administratives et médicales qui sont utilisées principalement pour le financement des établissements de santé (tarification à l’activité) et pour l’organisation de l’offre de soins (planification).</t>
-  </si>
-  <si>
-    <t>date_mis_a_jour_pmsi</t>
-  </si>
-  <si>
-    <t>date_mis_a_jour_finess</t>
-  </si>
-  <si>
-    <t>/</t>
-  </si>
-  <si>
-    <t>Source : ANCRE
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Source :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ANCRE
 Le plan comptable officiel des établissements publics de santé (EPS) et des établissements de santé privé d’intérêt collectif (ESPIC), dénommé M21, met à la disposition des gestionnaires un système commun de classification de budget qui permet ainsi d’affecter des dépenses à un budget défini.
 Le budget des hôpitaux publics s’organise dans le cadre d’un budget principal (activité hospitalière ou budget H) et, en fonction des activités assurées par les établissements, un ou plusieurs budgets annexes.
-Budget principal (Hospitalier) : il présente les opérations financières correspondant à l’activité sanitaire hors soins de longue durée des établissements de santé, couvrant le court et moyen séjour, l’hospitalisation à domicile et la psychiatrie.
-Budget annexe : distinct du budget principal, il présente les opérations financières relatives aux activités de soins de longue durée ou aux activités non sanitaires des hôpitaux publics, notamment des établissements d’hébergement pour personnes âgées dépendantes (Ehpad), des instituts de formation, des services de soins infirmiers à domicile (SSIAD), …
-Budget global : ensemble des budgets (budget principal et budgets annexes) du secteur public, consolidés des flux internes entre les différentes unités.
-Fréquence : Quotidienne
-Source(s) : ANCRE (Application Nationale Compte financier Rapport infra-annuel Eprd) - Agence technique de l’information sur l’hospitalisation (ATIH)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Budget principal (Hospitalier) :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> il présente les opérations financières correspondant à l’activité sanitaire hors soins de longue durée des établissements de santé, couvrant le court et moyen séjour, l’hospitalisation à domicile et la psychiatrie.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Budget annexe :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> distinct du budget principal, il présente les opérations financières relatives aux activités de soins de longue durée ou aux activités non sanitaires des hôpitaux publics, notamment des établissements d’hébergement pour personnes âgées dépendantes (Ehpad), des instituts de formation, des services de soins infirmiers à domicile (SSIAD), …
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Budget global :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ensemble des budgets (budget principal et budgets annexes) du secteur public, consolidés des flux internes entre les différentes unités.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Fréquence : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Quotidienne
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Source(s) : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ANCRE (Application Nationale Compte financier Rapport infra-annuel Eprd) - Agence technique de l’information sur l’hospitalisation (ATIH)
 Hélios collecte ces données depuis le SI mutualisé des ARS DIAMANT « Décisionnel Inter-ARS pour la Maîtrise et l’Anticipation. », outil décisionnel de pilotage centré sur la régulation de l’offre de soins, abordée sous les aspects des moyens humains, financiers, et productivité.</t>
-  </si>
-  <si>
-    <t>date_mis_a_jour_ancre</t>
-  </si>
-  <si>
-    <t>Source : ANCRE
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Source :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ANCRE
 Le résultat de l’exercice consiste en la différence entre les recettes/produits et les dépenses/charges comptabilisés au cours de l’exercice toutes activités confondues.
-Fréquence : Quotidienne
-Source(s) : ANCRE (Application Nationale Compte financier Rapport infra-annuel Eprd) - Agence technique de l’information sur l’hospitalisation (ATIH)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Fréquence :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Quotidienne
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Source(s) : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ANCRE (Application Nationale Compte financier Rapport infra-annuel Eprd) - Agence technique de l’information sur l’hospitalisation (ATIH)
 Hélios collecte ces données depuis le SI mutualisé des ARS DIAMANT « Décisionnel Inter-ARS pour la Maîtrise et l’Anticipation. », outil décisionnel de pilotage centré sur la régulation de l’offre de soins, abordée sous les aspects des moyens humains, financiers, et productivité.</t>
-  </si>
-  <si>
-    <t>Source : ANCRE
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Source : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">ANCRE
 Cet indicateur mesure la capacité de l’établissement à autofinancer ses investissements. Il mesure la part de CAF qui reste disponible après remboursement de l’annuité en capital de la dette. Une CAF &lt; 0 traduit une insuffisance d’autofinancement. Un taux de CAF inférieur à 2% est un critère de déséquilibre financier.
-Fréquence : Quotidienne
-Mode de calcul :
-Numérateur - Capacité d’autofinancement (CAF) :
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Fréquence : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Quotidienne
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Mode de calcul :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Numérateur - Capacité d’autofinancement (CAF) :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
 Annuité de remboursement du capital de la dette = Total des débits des comptes 16 « Emprunts et dettes assimilées », sauf 1688 "intérêts courus non échus" après retraitement des débits afférents aux renégociations d’emprunts, aux remboursements anticipés des emprunts et aux opérations de l’année sur les ouvertures de crédits long terme renouvelables (OCLTR) qui sont déduits de manière à obtenir l’« image » de l’annuité réelle de la dette, 166 « Refinancement de la dette » et 16449 « Opérations afférentes à l’option de tirage sur ligne de trésorerie ».
-Dénominateur - Solde des comptes :
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Dénominateur - Solde des comptes :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
 Produits d’exploitation (70 à 75 +781+791-sd709)
 + Produits financiers (76)
 + Produits exceptionnels (77 + 7874 + 7876 + 797)
 - 775 « Produits des cessions d’immobilisations »
 - 777 « Quote-part des subventions amortissables transférées au compte de résultat »
 - 78 « Reprises sur amortissements et provisions »
-Source(s) :
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Source(s) :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
 ANCRE (Application Nationale Compte financier Rapport infra-annuel Eprd) - Agence technique de l’information sur l’hospitalisation (ATIH)
 Hélios collecte ces données depuis le SI mutualisé des ARS DIAMANT « Décisionnel Inter-ARS pour la Maîtrise et l’Anticipation », outil décisionnel de pilotage centré sur la régulation de l’offre de soins, abordée sous les aspects des moyens humains, financiers, et productivité.</t>
-  </si>
-  <si>
-    <t>Source : ANCRE
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Source : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">ANCRE
 Cet indicateur mesure le poids que représente l’endettement de l’établissement dans les capitaux permanents (ressources du fonds de roulement hors amortissements et dépréciations). Un taux supérieur à 50% traduit une trop forte dépendance vis-à-vis des organismes prêteurs.
-Fréquence : Quotidienne
-Mode de calcul :
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Fréquence :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Quotidienne
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Mode de calcul :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
 Numérateur - Encours de la dette au 31.12.N
 Compte 163 « Emprunts obligataires » + Compte 164 « Emprunts auprès des établissements de crédit » + Comptes 165 à 168 « Emprunts et dettes financières divers » Les comptes 166 et 168 sont déduits.
 Dénominateur - Capitaux permanents
@@ -141,28 +588,138 @@
 + 163 « Emprunts obligataires »
 + 164 « Emprunts auprès des établissements de crédit »
 + 165 à 168 « Emprunts et dettes financières divers »
-Source(s) : ANCRE (Application Nationale Compte financier Rapport infra-annuel Eprd) - Agence technique de l’information sur l’hospitalisation (ATIH)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Source(s) : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ANCRE (Application Nationale Compte financier Rapport infra-annuel Eprd) - Agence technique de l’information sur l’hospitalisation (ATIH)
 Hélios collecte ces données depuis le SI mutualisé des ARS DIAMANT « Décisionnel Inter-ARS pour la Maîtrise et l’Anticipation. », outil décisionnel de pilotage centré sur la régulation de l’offre de soins, abordée sous les aspects des moyens humains, financiers, et productivité.</t>
-  </si>
-  <si>
-    <t>Source : HAPI
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Source :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> HAPI
 L’application HAPI « Autres champs » outille le processus de gestion et d’attribution des ressources liées aux enveloppes MIGAC, DAF, USLD, Forfait et FMESPP d’une part, et, le pilotage et l’ordonnancement des dépenses du fonds d’intervention régional (FIR) d’autre part.
-Mode de calcul :
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Mode de calcul :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
 Montant des crédits alloués par enveloppes, sous enveloppes et mode délégation, par campagne budgétaire.
-Fréquence : Quotidienne
-Source(s) : HAPI (HArmonisation et Partage d’Information) - Autres champs.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Fréquence :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Quotidienne
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Source(s) :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> HAPI (HArmonisation et Partage d’Information) - Autres champs.
 Hélios collecte ces données depuis le SI mutualisé des ARS DIAMANT « Décisionnel Inter-ARS pour la Maîtrise et l’Anticipation. », outil décisionnel de pilotage centré sur la régulation de l’offre de soins, abordée sous les aspects des moyens humains, financiers, et productivité.</t>
-  </si>
-  <si>
-    <t>date_mis_a_jour_hapi</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -550,7 +1107,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -558,18 +1115,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{587C9ED0-279B-44AC-9485-AC6832055B1B}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.25" style="2" customWidth="1"/>
+    <col min="1" max="1" width="21.19921875" style="2" customWidth="1"/>
     <col min="2" max="2" width="14.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="187.625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="187.59765625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -580,135 +1137,113 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="249.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>17</v>
+      <c r="B3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="252" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="185.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="3"/>
     </row>
-    <row r="7" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="156" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="3"/>
+      <c r="B7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="8" spans="1:3" ht="185.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="3"/>
+      <c r="B8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="9" spans="1:3" ht="157.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:3" ht="126" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="5"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="3"/>
+    </row>
+    <row r="10" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>20</v>
-      </c>
     </row>
-    <row r="10" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="126" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
+    <row r="11" spans="1:3" ht="85.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3"/>
       <c r="B11" s="4"/>
       <c r="C11" s="3"/>
     </row>
-    <row r="12" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="3"/>
-    </row>
-    <row r="14" spans="1:3" ht="236.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>23</v>
+    <row r="12" spans="1:3" ht="234" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="C5:C8"/>
-    <mergeCell ref="B5:B8"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="A10:A11"/>
+    <mergeCell ref="C3:C6"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A8:A9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
(hel-839) fix: problème d'affichae mineurs dans excel
</commit_message>
<xml_diff>
--- a/public/templates/template_comparaison_EJ.xlsx
+++ b/public/templates/template_comparaison_EJ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Debian\home\webadm\projets\helios\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F70098A-629F-4F51-9E2F-6AB3DD524889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC050F3-0113-406E-86F1-8F0B3C6BF03B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -159,142 +159,6 @@
 Hospitalisation A Domicile (HAD) - fichiers RAPSS (Résumés Anonyme Par Sous-Séquence)
 Hélios collecte ces données depuis le SI mutualisé des ARS DIAMANT « Décisionnel Inter-ARS pour la Maîtrise et l’Anticipation. », outil décisionnel de pilotage centré sur la régulation de l’offre de soins, abordée sous les aspects des moyens humains, financiers, et productivité.
 Dans le cadre du PMSI, tout séjour dans un établissement de santé, public ou privé, fait l’objet d’un recueil systématique et minimal d’informations administratives et médicales qui sont utilisées principalement pour le financement des établissements de santé (tarification à l’activité) et pour l’organisation de l’offre de soins (planification).</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Source :</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ANCRE
-Le plan comptable officiel des établissements publics de santé (EPS) et des établissements de santé privé d’intérêt collectif (ESPIC), dénommé M21, met à la disposition des gestionnaires un système commun de classification de budget qui permet ainsi d’affecter des dépenses à un budget défini.
-Le budget des hôpitaux publics s’organise dans le cadre d’un budget principal (activité hospitalière ou budget H) et, en fonction des activités assurées par les établissements, un ou plusieurs budgets annexes.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Budget principal (Hospitalier) :</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> il présente les opérations financières correspondant à l’activité sanitaire hors soins de longue durée des établissements de santé, couvrant le court et moyen séjour, l’hospitalisation à domicile et la psychiatrie.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Budget annexe :</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> distinct du budget principal, il présente les opérations financières relatives aux activités de soins de longue durée ou aux activités non sanitaires des hôpitaux publics, notamment des établissements d’hébergement pour personnes âgées dépendantes (Ehpad), des instituts de formation, des services de soins infirmiers à domicile (SSIAD), …
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Budget global :</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ensemble des budgets (budget principal et budgets annexes) du secteur public, consolidés des flux internes entre les différentes unités.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Fréquence : </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Quotidienne
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Source(s) : </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ANCRE (Application Nationale Compte financier Rapport infra-annuel Eprd) - Agence technique de l’information sur l’hospitalisation (ATIH)
-Hélios collecte ces données depuis le SI mutualisé des ARS DIAMANT « Décisionnel Inter-ARS pour la Maîtrise et l’Anticipation. », outil décisionnel de pilotage centré sur la régulation de l’offre de soins, abordée sous les aspects des moyens humains, financiers, et productivité.</t>
     </r>
   </si>
   <si>
@@ -703,6 +567,143 @@
       </rPr>
       <t xml:space="preserve"> HAPI (HArmonisation et Partage d’Information) - Autres champs.
 Hélios collecte ces données depuis le SI mutualisé des ARS DIAMANT « Décisionnel Inter-ARS pour la Maîtrise et l’Anticipation. », outil décisionnel de pilotage centré sur la régulation de l’offre de soins, abordée sous les aspects des moyens humains, financiers, et productivité.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Source :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ANCRE
+Le plan comptable officiel des établissements publics de santé (EPS) et des établissements de santé privé d’intérêt collectif (ESPIC), dénommé M21, met à la disposition des gestionnaires un système commun de classification de budget qui permet ainsi d’affecter des dépenses à un budget défini.
+Le budget des hôpitaux publics s’organise dans le cadre d’un budget principal (activité hospitalière ou budget H) et, en fonction des activités assurées par les établissements, un ou plusieurs budgets annexes.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Budget principal (Hospitalier) :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> il présente les opérations financières correspondant à l’activité sanitaire hors soins de longue durée des établissements de santé, couvrant le court et moyen séjour, l’hospitalisation à domicile et la psychiatrie.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Budget annexe :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> distinct du budget principal, il présente les opérations financières relatives aux activités de soins de longue durée ou aux activités non sanitaires des hôpitaux publics, notamment des établissements d’hébergement pour personnes âgées dépendantes (Ehpad), des instituts de formation, des services de soins infirmiers à domicile (SSIAD), …
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Budget global :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ensemble des budgets (budget principal et budgets annexes) du secteur public, consolidés des flux internes entre les différentes unités.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Fréquence : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Quotidienne
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Source(s) : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">ANCRE (Application Nationale Compte financier Rapport infra-annuel Eprd) - Agence technique de l’information sur l’hospitalisation (ATIH)
+Hélios collecte ces données depuis le SI mutualisé des ARS DIAMANT « Décisionnel Inter-ARS pour la Maîtrise et l’Anticipation. », outil décisionnel de pilotage centré sur la régulation de l’offre de soins, abordée sous les aspects des moyens humains, financiers, et productivité.
+</t>
     </r>
   </si>
 </sst>
@@ -1156,7 +1157,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
@@ -1173,7 +1174,7 @@
       <c r="B5" s="4"/>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:3" ht="185.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="188.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -1188,7 +1189,7 @@
         <v>13</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1199,7 +1200,7 @@
         <v>13</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="126" customHeight="1" x14ac:dyDescent="0.3">
@@ -1215,10 +1216,10 @@
         <v>13</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="85.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="4"/>
       <c r="C11" s="3"/>
@@ -1231,7 +1232,7 @@
         <v>14</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
(hel-839) prise en compte des retours PR et démo
</commit_message>
<xml_diff>
--- a/public/templates/template_comparaison_EJ.xlsx
+++ b/public/templates/template_comparaison_EJ.xlsx
@@ -1,22 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29311"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Debian\home\webadm\projets\helios\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC050F3-0113-406E-86F1-8F0B3C6BF03B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{4FC050F3-0113-406E-86F1-8F0B3C6BF03B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA6D9428-9DD4-4E1F-B9F3-FC8895F1EAB1}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Comparaison" sheetId="1" r:id="rId1"/>
-    <sheet name="Lisez-moi" sheetId="2" r:id="rId2"/>
+    <sheet name="Lisez-moi" sheetId="2" r:id="rId1"/>
+    <sheet name="Comparaison" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -26,46 +42,16 @@
     <t>Indicateurs</t>
   </si>
   <si>
+    <t>Mise à jour</t>
+  </si>
+  <si>
     <t>Détails de l'indicateur</t>
   </si>
   <si>
-    <t>Mise à jour</t>
-  </si>
-  <si>
     <t>Nb de séjours HAD</t>
   </si>
   <si>
-    <t>Compte de résultat - Charges  (Budgets principaux)</t>
-  </si>
-  <si>
-    <t>Compte de résultat - Charges  (Budgets Annexes)</t>
-  </si>
-  <si>
-    <t>Compte de résultat - Produits (Budgets principaux)</t>
-  </si>
-  <si>
-    <t>Compte de résultat - Produits (Budgets Annexes)</t>
-  </si>
-  <si>
-    <t>Résultat net comptable</t>
-  </si>
-  <si>
-    <t>Taux de CAF</t>
-  </si>
-  <si>
-    <t>Ratio de dépendance financière</t>
-  </si>
-  <si>
-    <t>Allocation de ressources</t>
-  </si>
-  <si>
     <t>date_mis_a_jour_pmsi</t>
-  </si>
-  <si>
-    <t>date_mis_a_jour_ancre</t>
-  </si>
-  <si>
-    <t>date_mis_a_jour_hapi</t>
   </si>
   <si>
     <r>
@@ -162,6 +148,161 @@
     </r>
   </si>
   <si>
+    <t>Compte de résultat - Charges  (Budgets principaux)</t>
+  </si>
+  <si>
+    <t>date_mis_a_jour_ancre</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Source :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ANCRE
+Le plan comptable officiel des établissements publics de santé (EPS) et des établissements de santé privé d’intérêt collectif (ESPIC), dénommé M21, met à la disposition des gestionnaires un système commun de classification de budget qui permet ainsi d’affecter des dépenses à un budget défini.
+Le budget des hôpitaux publics s’organise dans le cadre d’un budget principal (activité hospitalière ou budget H) et, en fonction des activités assurées par les établissements, un ou plusieurs budgets annexes.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Budget principal (Hospitalier) :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> il présente les opérations financières correspondant à l’activité sanitaire hors soins de longue durée des établissements de santé, couvrant le court et moyen séjour, l’hospitalisation à domicile et la psychiatrie.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Budget annexe :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> distinct du budget principal, il présente les opérations financières relatives aux activités de soins de longue durée ou aux activités non sanitaires des hôpitaux publics, notamment des établissements d’hébergement pour personnes âgées dépendantes (Ehpad), des instituts de formation, des services de soins infirmiers à domicile (SSIAD), …
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Budget global :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ensemble des budgets (budget principal et budgets annexes) du secteur public, consolidés des flux internes entre les différentes unités.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Fréquence : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Quotidienne
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Source(s) : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">ANCRE (Application Nationale Compte financier Rapport infra-annuel Eprd) - Agence technique de l’information sur l’hospitalisation (ATIH)
+Hélios collecte ces données depuis le SI mutualisé des ARS DIAMANT « Décisionnel Inter-ARS pour la Maîtrise et l’Anticipation. », outil décisionnel de pilotage centré sur la régulation de l’offre de soins, abordée sous les aspects des moyens humains, financiers, et productivité.
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Compte de résultat - Charges  (Budgets Annexes)</t>
+  </si>
+  <si>
+    <t>Compte de résultat - Produits (Budgets principaux)</t>
+  </si>
+  <si>
+    <t>Compte de résultat - Produits (Budgets Annexes)</t>
+  </si>
+  <si>
+    <t>Résultat net comptable</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -229,6 +370,9 @@
       <t>ANCRE (Application Nationale Compte financier Rapport infra-annuel Eprd) - Agence technique de l’information sur l’hospitalisation (ATIH)
 Hélios collecte ces données depuis le SI mutualisé des ARS DIAMANT « Décisionnel Inter-ARS pour la Maîtrise et l’Anticipation. », outil décisionnel de pilotage centré sur la régulation de l’offre de soins, abordée sous les aspects des moyens humains, financiers, et productivité.</t>
     </r>
+  </si>
+  <si>
+    <t>Taux de CAF</t>
   </si>
   <si>
     <r>
@@ -372,6 +516,9 @@
 ANCRE (Application Nationale Compte financier Rapport infra-annuel Eprd) - Agence technique de l’information sur l’hospitalisation (ATIH)
 Hélios collecte ces données depuis le SI mutualisé des ARS DIAMANT « Décisionnel Inter-ARS pour la Maîtrise et l’Anticipation », outil décisionnel de pilotage centré sur la régulation de l’offre de soins, abordée sous les aspects des moyens humains, financiers, et productivité.</t>
     </r>
+  </si>
+  <si>
+    <t>Ratio de dépendance financière</t>
   </si>
   <si>
     <r>
@@ -478,6 +625,12 @@
     </r>
   </si>
   <si>
+    <t>Allocation de ressources</t>
+  </si>
+  <si>
+    <t>date_mis_a_jour_hapi</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -567,143 +720,6 @@
       </rPr>
       <t xml:space="preserve"> HAPI (HArmonisation et Partage d’Information) - Autres champs.
 Hélios collecte ces données depuis le SI mutualisé des ARS DIAMANT « Décisionnel Inter-ARS pour la Maîtrise et l’Anticipation. », outil décisionnel de pilotage centré sur la régulation de l’offre de soins, abordée sous les aspects des moyens humains, financiers, et productivité.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Source :</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ANCRE
-Le plan comptable officiel des établissements publics de santé (EPS) et des établissements de santé privé d’intérêt collectif (ESPIC), dénommé M21, met à la disposition des gestionnaires un système commun de classification de budget qui permet ainsi d’affecter des dépenses à un budget défini.
-Le budget des hôpitaux publics s’organise dans le cadre d’un budget principal (activité hospitalière ou budget H) et, en fonction des activités assurées par les établissements, un ou plusieurs budgets annexes.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Budget principal (Hospitalier) :</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> il présente les opérations financières correspondant à l’activité sanitaire hors soins de longue durée des établissements de santé, couvrant le court et moyen séjour, l’hospitalisation à domicile et la psychiatrie.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Budget annexe :</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> distinct du budget principal, il présente les opérations financières relatives aux activités de soins de longue durée ou aux activités non sanitaires des hôpitaux publics, notamment des établissements d’hébergement pour personnes âgées dépendantes (Ehpad), des instituts de formation, des services de soins infirmiers à domicile (SSIAD), …
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Budget global :</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ensemble des budgets (budget principal et budgets annexes) du secteur public, consolidés des flux internes entre les différentes unités.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Fréquence : </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Quotidienne
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Source(s) : </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">ANCRE (Application Nationale Compte financier Rapport infra-annuel Eprd) - Agence technique de l’information sur l’hospitalisation (ATIH)
-Hélios collecte ces données depuis le SI mutualisé des ARS DIAMANT « Décisionnel Inter-ARS pour la Maîtrise et l’Anticipation. », outil décisionnel de pilotage centré sur la régulation de l’offre de soins, abordée sous les aspects des moyens humains, financiers, et productivité.
-</t>
     </r>
   </si>
 </sst>
@@ -711,7 +727,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1103,136 +1119,124 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{587C9ED0-279B-44AC-9485-AC6832055B1B}">
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="21.19921875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="21.25" style="2" customWidth="1"/>
     <col min="2" max="2" width="14.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="187.59765625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="187.625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
     </row>
-    <row r="2" spans="1:3" ht="249.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="262.5" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="46.9">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="46.9">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="46.9">
       <c r="A5" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:3" ht="188.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="188.45" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="3"/>
     </row>
-    <row r="7" spans="1:3" ht="156" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="180" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>16</v>
-      </c>
     </row>
-    <row r="8" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="409.5" customHeight="1">
       <c r="A8" s="5" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="126" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="144" customHeight="1">
       <c r="A9" s="5"/>
       <c r="B9" s="4"/>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="409.5" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="100.15" customHeight="1">
       <c r="A11" s="3"/>
       <c r="B11" s="4"/>
       <c r="C11" s="3"/>
     </row>
-    <row r="12" spans="1:3" ht="234" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="257.25" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1249,4 +1253,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
(hel-888) description pour indicateur Allocation Ress EJ et ETSAN Excel de comparaison
</commit_message>
<xml_diff>
--- a/public/templates/template_comparaison_EJ.xlsx
+++ b/public/templates/template_comparaison_EJ.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29322"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Debian\home\webadm\projets\helios\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{4FC050F3-0113-406E-86F1-8F0B3C6BF03B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA6D9428-9DD4-4E1F-B9F3-FC8895F1EAB1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1007A4AD-03A1-49A6-9C75-414404E5FC40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lisez-moi" sheetId="2" r:id="rId1"/>
@@ -635,9 +635,8 @@
       <rPr>
         <b/>
         <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
       <t>Source :</t>
@@ -645,12 +644,12 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> HAPI
+Pour la campagne et le type d’établissement sélectionnés, cette enveloppe fait partie des 3 premières enveloppes attribuées.
 L’application HAPI « Autres champs » outille le processus de gestion et d’attribution des ressources liées aux enveloppes MIGAC, DAF, USLD, Forfait et FMESPP d’une part, et, le pilotage et l’ordonnancement des dépenses du fonds d’intervention régional (FIR) d’autre part.
 </t>
     </r>
@@ -658,19 +657,18 @@
       <rPr>
         <b/>
         <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Mode de calcul :</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Mode de calcul :
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
@@ -681,9 +679,8 @@
       <rPr>
         <b/>
         <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
       <t>Fréquence :</t>
@@ -691,9 +688,8 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> Quotidienne
@@ -703,9 +699,8 @@
       <rPr>
         <b/>
         <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
       <t>Source(s) :</t>
@@ -713,9 +708,8 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> HAPI (HArmonisation et Partage d’Information) - Autres champs.
@@ -727,7 +721,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -741,6 +735,19 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -772,14 +779,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1157,10 +1164,10 @@
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1168,22 +1175,22 @@
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="3"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="4"/>
     </row>
     <row r="5" spans="1:3" ht="46.9">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="3"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="4"/>
     </row>
     <row r="6" spans="1:3" ht="188.45" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="3"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="4"/>
     </row>
     <row r="7" spans="1:3" ht="180" customHeight="1">
       <c r="A7" s="2" t="s">
@@ -1197,36 +1204,36 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="409.5" customHeight="1">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="144" customHeight="1">
-      <c r="A9" s="5"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="3"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="4"/>
     </row>
     <row r="10" spans="1:3" ht="409.5" customHeight="1">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="100.15" customHeight="1">
-      <c r="A11" s="3"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="3"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="4"/>
     </row>
     <row r="12" spans="1:3" ht="257.25" customHeight="1">
       <c r="A12" s="2" t="s">
@@ -1235,7 +1242,7 @@
       <c r="B12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="3" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1262,7 +1269,9 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" customFormat="1" ht="15.75"/>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
(hel-888) description pour indicateur Allocation Ress EJ et ETSAN Excel de comparaison (#847)
</commit_message>
<xml_diff>
--- a/public/templates/template_comparaison_EJ.xlsx
+++ b/public/templates/template_comparaison_EJ.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29322"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Debian\home\webadm\projets\helios\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{4FC050F3-0113-406E-86F1-8F0B3C6BF03B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA6D9428-9DD4-4E1F-B9F3-FC8895F1EAB1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1007A4AD-03A1-49A6-9C75-414404E5FC40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lisez-moi" sheetId="2" r:id="rId1"/>
@@ -635,9 +635,8 @@
       <rPr>
         <b/>
         <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
       <t>Source :</t>
@@ -645,12 +644,12 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> HAPI
+Pour la campagne et le type d’établissement sélectionnés, cette enveloppe fait partie des 3 premières enveloppes attribuées.
 L’application HAPI « Autres champs » outille le processus de gestion et d’attribution des ressources liées aux enveloppes MIGAC, DAF, USLD, Forfait et FMESPP d’une part, et, le pilotage et l’ordonnancement des dépenses du fonds d’intervention régional (FIR) d’autre part.
 </t>
     </r>
@@ -658,19 +657,18 @@
       <rPr>
         <b/>
         <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Mode de calcul :</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Mode de calcul :
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
@@ -681,9 +679,8 @@
       <rPr>
         <b/>
         <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
       <t>Fréquence :</t>
@@ -691,9 +688,8 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> Quotidienne
@@ -703,9 +699,8 @@
       <rPr>
         <b/>
         <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
       <t>Source(s) :</t>
@@ -713,9 +708,8 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> HAPI (HArmonisation et Partage d’Information) - Autres champs.
@@ -727,7 +721,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -741,6 +735,19 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -772,14 +779,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1157,10 +1164,10 @@
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1168,22 +1175,22 @@
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="3"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="4"/>
     </row>
     <row r="5" spans="1:3" ht="46.9">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="3"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="4"/>
     </row>
     <row r="6" spans="1:3" ht="188.45" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="3"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="4"/>
     </row>
     <row r="7" spans="1:3" ht="180" customHeight="1">
       <c r="A7" s="2" t="s">
@@ -1197,36 +1204,36 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="409.5" customHeight="1">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="144" customHeight="1">
-      <c r="A9" s="5"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="3"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="4"/>
     </row>
     <row r="10" spans="1:3" ht="409.5" customHeight="1">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="100.15" customHeight="1">
-      <c r="A11" s="3"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="3"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="4"/>
     </row>
     <row r="12" spans="1:3" ht="257.25" customHeight="1">
       <c r="A12" s="2" t="s">
@@ -1235,7 +1242,7 @@
       <c r="B12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="3" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1262,7 +1269,9 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" customFormat="1" ht="15.75"/>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
(hel-917) Prise en compte des nouvelles valeurs dans l’export
</commit_message>
<xml_diff>
--- a/public/templates/template_comparaison_EJ.xlsx
+++ b/public/templates/template_comparaison_EJ.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29322"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Debian\home\webadm\projets\helios\public\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://catamaniacrm-my.sharepoint.com/personal/y_elhouakmi_catamania_com/Documents/Documents/DNum/Helios/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1007A4AD-03A1-49A6-9C75-414404E5FC40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="8_{1007A4AD-03A1-49A6-9C75-414404E5FC40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2DB7AABD-2764-44C4-8FAA-27989E0C030D}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lisez-moi" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
   <si>
     <t>Indicateurs</t>
   </si>
@@ -716,12 +716,377 @@
 Hélios collecte ces données depuis le SI mutualisé des ARS DIAMANT « Décisionnel Inter-ARS pour la Maîtrise et l’Anticipation. », outil décisionnel de pilotage centré sur la régulation de l’offre de soins, abordée sous les aspects des moyens humains, financiers, et productivité.</t>
     </r>
   </si>
+  <si>
+    <t>Nb ETP PM</t>
+  </si>
+  <si>
+    <t>Nb ETP PNM</t>
+  </si>
+  <si>
+    <t>Dépenses intérim PM</t>
+  </si>
+  <si>
+    <t>Jours d’absentéisme PM</t>
+  </si>
+  <si>
+    <t>Jours d’absentéisme PNM</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Fréquence</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : Quotidienne
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Mode de calcul :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Nombre d’équivalents temps pleins moyens rémunérés personnel médical
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Source(s) :
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Application Nationale Compte financier Rapport infra-annuel Eprd (ANCRE) - Agence technique de l’information sur l’hospitalisation (ATIH)
+Fichier de la campagne CF.
+Hélios collecte ces données depuis le SI mutualisé des ARS DIAMANT qui est un système décisionnel national permettant de stocker des informations provenant de plusieurs sources. DIAMANT : Décisionnel Inter-ARS pour la Maîtrise et l’Anticipation.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Fréquence :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Quotidienne
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Mode de calcul : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Nombre d’équivalents temps pleins moyens rémunérés personnel non médical
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Source(s) :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Application Nationale Compte financier Rapport infra-annuel Eprd (ANCRE) - Agence technique de l’information sur l’hospitalisation (ATIH)
+Fichier de la campagne CF.
+Hélios collecte ces données depuis le SI mutualisé des ARS DIAMANT qui est un système décisionnel national permettant de stocker des informations provenant de plusieurs sources. DIAMANT : Décisionnel Inter-ARS pour la Maîtrise et l’Anticipation.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Fréquence :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Quotidienne
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Mode de calcul : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Montant du compte de charge "62113 Personnel intérimaire médical"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Source(s) :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Application Nationale Compte financier Rapport infra-annuel Eprd (ANCRE) - Agence technique de l’information sur l’hospitalisation (ATIH)
+Fichier de la campagne CF.
+Hélios collecte ces données depuis le SI mutualisé des ARS DIAMANT qui est un système décisionnel national permettant de stocker des informations provenant de plusieurs sources. DIAMANT : Décisionnel Inter-ARS pour la Maîtrise et l’Anticipation.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Fréquence :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Quotidienne
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Mode de calcul : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Nombre de jours d’absence du personnel médical
+La réalisation du bilan social est obligatoire pour les établissements (qu’ils soient sanitaires, sociaux ou médico-sociaux) dont l’effectif global au 31/12/n-1 est d’au moins 300 agents. Il est facultatif pour les autres établissements.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Source(s) :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Enquête « Bilan Social »- Agence technique de l’information sur l’hospitalisation (ATIH)
+Hélios collecte ces données depuis le SI mutualisé des ARS DIAMANT qui est un système décisionnel national permettant de stocker des informations provenant de plusieurs sources. DIAMANT : Décisionnel Inter-ARS pour la Maîtrise et l’Anticipation.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Fréquence :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Quotidienne
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Mode de calcul : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Nombre de jours d’absence du personnel non médical
+La réalisation du bilan social est obligatoire pour les établissements (qu’ils soient sanitaires, sociaux ou médico-sociaux) dont l’effectif global au 31/12/n-1 est d’au moins 300 agents. Il est facultatif pour les autres établissements.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Source(s) :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Enquête « Bilan Social »- Agence technique de l’information sur l’hospitalisation (ATIH)
+Hélios collecte ces données depuis le SI mutualisé des ARS DIAMANT qui est un système décisionnel national permettant de stocker des informations provenant de plusieurs sources. DIAMANT : Décisionnel Inter-ARS pour la Maîtrise et l’Anticipation.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -771,7 +1136,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -787,6 +1152,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1127,18 +1495,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{587C9ED0-279B-44AC-9485-AC6832055B1B}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.25" style="2" customWidth="1"/>
-    <col min="2" max="2" width="14.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="187.625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1149,7 +1517,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="262.5" customHeight="1">
+    <row r="2" spans="1:3" ht="262.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -1160,102 +1528,157 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="46.9">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:3" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="173.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="173.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="46.9">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="4"/>
-    </row>
-    <row r="5" spans="1:3" ht="46.9">
-      <c r="A5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="4"/>
-    </row>
-    <row r="6" spans="1:3" ht="188.45" customHeight="1">
-      <c r="A6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="4"/>
-    </row>
-    <row r="7" spans="1:3" ht="180" customHeight="1">
-      <c r="A7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="409.5" customHeight="1">
-      <c r="A8" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="144" customHeight="1">
-      <c r="A9" s="4"/>
+    <row r="9" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="B9" s="5"/>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:3" ht="409.5" customHeight="1">
-      <c r="A10" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>17</v>
-      </c>
+    <row r="10" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:3" ht="100.15" customHeight="1">
-      <c r="A11" s="4"/>
+    <row r="11" spans="1:3" ht="188.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="B11" s="5"/>
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:3" ht="257.25" customHeight="1">
+    <row r="12" spans="1:3" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="144" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="4"/>
+    </row>
+    <row r="15" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="4"/>
+    </row>
+    <row r="17" spans="1:3" ht="257.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="C3:C6"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="C8:C11"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A13:A14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1268,10 +1691,8 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
-  <sheetData>
-    <row r="1" customFormat="1" ht="15.75"/>
-  </sheetData>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Hel 917/ajout indicateur comparaison ej (#925)
* (hel-917) Ajout des informations RH à la comparaison EJ

* (hel-917) Formattage des valeurs

* (hel-917) Ajout de l’infobulle

* (hel-917) Prise en compte des nouvelles valeurs dans l’export

* (hel-917) Prise en compte des nouvelles variables dans les tests

* (hel-917) Correction retour PR

* (hel-917) Fix sonarlint
</commit_message>
<xml_diff>
--- a/public/templates/template_comparaison_EJ.xlsx
+++ b/public/templates/template_comparaison_EJ.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29322"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Debian\home\webadm\projets\helios\public\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://catamaniacrm-my.sharepoint.com/personal/y_elhouakmi_catamania_com/Documents/Documents/DNum/Helios/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1007A4AD-03A1-49A6-9C75-414404E5FC40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="8_{1007A4AD-03A1-49A6-9C75-414404E5FC40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2DB7AABD-2764-44C4-8FAA-27989E0C030D}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lisez-moi" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
   <si>
     <t>Indicateurs</t>
   </si>
@@ -716,12 +716,377 @@
 Hélios collecte ces données depuis le SI mutualisé des ARS DIAMANT « Décisionnel Inter-ARS pour la Maîtrise et l’Anticipation. », outil décisionnel de pilotage centré sur la régulation de l’offre de soins, abordée sous les aspects des moyens humains, financiers, et productivité.</t>
     </r>
   </si>
+  <si>
+    <t>Nb ETP PM</t>
+  </si>
+  <si>
+    <t>Nb ETP PNM</t>
+  </si>
+  <si>
+    <t>Dépenses intérim PM</t>
+  </si>
+  <si>
+    <t>Jours d’absentéisme PM</t>
+  </si>
+  <si>
+    <t>Jours d’absentéisme PNM</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Fréquence</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : Quotidienne
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Mode de calcul :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Nombre d’équivalents temps pleins moyens rémunérés personnel médical
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Source(s) :
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Application Nationale Compte financier Rapport infra-annuel Eprd (ANCRE) - Agence technique de l’information sur l’hospitalisation (ATIH)
+Fichier de la campagne CF.
+Hélios collecte ces données depuis le SI mutualisé des ARS DIAMANT qui est un système décisionnel national permettant de stocker des informations provenant de plusieurs sources. DIAMANT : Décisionnel Inter-ARS pour la Maîtrise et l’Anticipation.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Fréquence :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Quotidienne
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Mode de calcul : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Nombre d’équivalents temps pleins moyens rémunérés personnel non médical
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Source(s) :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Application Nationale Compte financier Rapport infra-annuel Eprd (ANCRE) - Agence technique de l’information sur l’hospitalisation (ATIH)
+Fichier de la campagne CF.
+Hélios collecte ces données depuis le SI mutualisé des ARS DIAMANT qui est un système décisionnel national permettant de stocker des informations provenant de plusieurs sources. DIAMANT : Décisionnel Inter-ARS pour la Maîtrise et l’Anticipation.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Fréquence :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Quotidienne
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Mode de calcul : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Montant du compte de charge "62113 Personnel intérimaire médical"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Source(s) :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Application Nationale Compte financier Rapport infra-annuel Eprd (ANCRE) - Agence technique de l’information sur l’hospitalisation (ATIH)
+Fichier de la campagne CF.
+Hélios collecte ces données depuis le SI mutualisé des ARS DIAMANT qui est un système décisionnel national permettant de stocker des informations provenant de plusieurs sources. DIAMANT : Décisionnel Inter-ARS pour la Maîtrise et l’Anticipation.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Fréquence :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Quotidienne
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Mode de calcul : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Nombre de jours d’absence du personnel médical
+La réalisation du bilan social est obligatoire pour les établissements (qu’ils soient sanitaires, sociaux ou médico-sociaux) dont l’effectif global au 31/12/n-1 est d’au moins 300 agents. Il est facultatif pour les autres établissements.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Source(s) :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Enquête « Bilan Social »- Agence technique de l’information sur l’hospitalisation (ATIH)
+Hélios collecte ces données depuis le SI mutualisé des ARS DIAMANT qui est un système décisionnel national permettant de stocker des informations provenant de plusieurs sources. DIAMANT : Décisionnel Inter-ARS pour la Maîtrise et l’Anticipation.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Fréquence :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Quotidienne
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Mode de calcul : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Nombre de jours d’absence du personnel non médical
+La réalisation du bilan social est obligatoire pour les établissements (qu’ils soient sanitaires, sociaux ou médico-sociaux) dont l’effectif global au 31/12/n-1 est d’au moins 300 agents. Il est facultatif pour les autres établissements.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Source(s) :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Enquête « Bilan Social »- Agence technique de l’information sur l’hospitalisation (ATIH)
+Hélios collecte ces données depuis le SI mutualisé des ARS DIAMANT qui est un système décisionnel national permettant de stocker des informations provenant de plusieurs sources. DIAMANT : Décisionnel Inter-ARS pour la Maîtrise et l’Anticipation.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -771,7 +1136,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -787,6 +1152,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1127,18 +1495,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{587C9ED0-279B-44AC-9485-AC6832055B1B}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.25" style="2" customWidth="1"/>
-    <col min="2" max="2" width="14.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="187.625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1149,7 +1517,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="262.5" customHeight="1">
+    <row r="2" spans="1:3" ht="262.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -1160,102 +1528,157 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="46.9">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:3" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="173.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="173.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="46.9">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="4"/>
-    </row>
-    <row r="5" spans="1:3" ht="46.9">
-      <c r="A5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="4"/>
-    </row>
-    <row r="6" spans="1:3" ht="188.45" customHeight="1">
-      <c r="A6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="4"/>
-    </row>
-    <row r="7" spans="1:3" ht="180" customHeight="1">
-      <c r="A7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="409.5" customHeight="1">
-      <c r="A8" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="144" customHeight="1">
-      <c r="A9" s="4"/>
+    <row r="9" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="B9" s="5"/>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:3" ht="409.5" customHeight="1">
-      <c r="A10" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>17</v>
-      </c>
+    <row r="10" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:3" ht="100.15" customHeight="1">
-      <c r="A11" s="4"/>
+    <row r="11" spans="1:3" ht="188.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="B11" s="5"/>
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:3" ht="257.25" customHeight="1">
+    <row r="12" spans="1:3" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="144" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="4"/>
+    </row>
+    <row r="15" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="4"/>
+    </row>
+    <row r="17" spans="1:3" ht="257.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="C3:C6"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="C8:C11"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A13:A14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1268,10 +1691,8 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
-  <sheetData>
-    <row r="1" customFormat="1" ht="15.75"/>
-  </sheetData>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>